<commit_message>
resolved unauthorized error when try to login
</commit_message>
<xml_diff>
--- a/reports/Branch_Transactions_undefined.xlsx
+++ b/reports/Branch_Transactions_undefined.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
   <si>
     <t>Farmer Name</t>
   </si>
@@ -34,10 +34,10 @@
     <t>RajaBhau Patil</t>
   </si>
   <si>
-    <t>1234567890</t>
-  </si>
-  <si>
-    <t>2025-04-03</t>
+    <t>9420208901</t>
+  </si>
+  <si>
+    <t>2025-03-26</t>
   </si>
   <si>
     <t>Cow</t>
@@ -423,7 +423,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="20" customWidth="1"/>
@@ -461,32 +461,12 @@
         <v>8</v>
       </c>
       <c r="D2">
-        <v>8.4</v>
+        <v>780</v>
       </c>
       <c r="E2">
-        <v>1</v>
+        <v>150</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C3" t="s">
-        <v>8</v>
-      </c>
-      <c r="D3">
-        <v>700</v>
-      </c>
-      <c r="E3">
-        <v>100</v>
-      </c>
-      <c r="F3" t="s">
         <v>9</v>
       </c>
     </row>

</xml_diff>